<commit_message>
Disable stability criteria in the test of PLBVFU1. Reduce disturbance in PLBVF data.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/plbvf.xlsx
+++ b/andes/cases/ieee14/plbvf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/ieee14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hacui\repos\andes\andes\cases\ieee14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE26CFB-4D87-4444-8D83-A768C2A8F4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC1E28-EA59-466E-BA00-032A8DCBF56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="5160" windowWidth="16560" windowHeight="11600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="2220" windowWidth="12000" windowHeight="16530" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLBVF" sheetId="1" r:id="rId1"/>
@@ -387,13 +387,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -415,7 +415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.2</v>
       </c>
@@ -423,10 +423,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.4</v>
       </c>
@@ -434,10 +434,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.6</v>
       </c>
@@ -445,10 +445,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.8</v>
       </c>
@@ -456,10 +456,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -467,10 +467,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -489,10 +489,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.6</v>
       </c>
@@ -500,10 +500,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C10" s="1">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1.8</v>
       </c>
@@ -511,10 +511,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -522,10 +522,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="1">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -533,10 +533,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2.4</v>
       </c>

</xml_diff>

<commit_message>
Reduce the magnitude of disturbances.
</commit_message>
<xml_diff>
--- a/andes/cases/ieee14/plbvf.xlsx
+++ b/andes/cases/ieee14/plbvf.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/ieee14/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\hacui\repos\andes\andes\cases\ieee14\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACE26CFB-4D87-4444-8D83-A768C2A8F4D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39EC1E28-EA59-466E-BA00-032A8DCBF56A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29340" yWindow="5160" windowWidth="16560" windowHeight="11600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19080" yWindow="2220" windowWidth="12000" windowHeight="16530" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLBVF" sheetId="1" r:id="rId1"/>
@@ -387,13 +387,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -404,7 +404,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -415,7 +415,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>0.2</v>
       </c>
@@ -423,10 +423,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C3" s="1">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>0.4</v>
       </c>
@@ -434,10 +434,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C4" s="1">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>0.6</v>
       </c>
@@ -445,10 +445,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C5" s="1">
-        <v>1.03</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0029999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>0.8</v>
       </c>
@@ -456,10 +456,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C6" s="1">
-        <v>1.02</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>1</v>
       </c>
@@ -467,10 +467,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>1.01</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+        <v>1.0009999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>1.2</v>
       </c>
@@ -481,7 +481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>1.4</v>
       </c>
@@ -489,10 +489,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C9" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>1.6</v>
       </c>
@@ -500,10 +500,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C10" s="1">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>1.8</v>
       </c>
@@ -511,10 +511,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C11" s="1">
-        <v>0.97</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -522,10 +522,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C12" s="1">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>2.2000000000000002</v>
       </c>
@@ -533,10 +533,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="C13" s="1">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>2.4</v>
       </c>

</xml_diff>